<commit_message>
creat Excel for all course
</commit_message>
<xml_diff>
--- a/registered_courses.xlsx
+++ b/registered_courses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>0924295880</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -496,82 +496,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>مراقبت زیبایی</t>
+          <t>خیاطی</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1402/11/23</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>tina</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>amini</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>09916450191</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>حسابداری</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>1402/11/23</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>tina</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>amini</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>09916450191</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>خیاطی</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>1402/11/23</t>
+          <t>1402/11/25</t>
         </is>
       </c>
     </row>

</xml_diff>